<commit_message>
Implementación de ciclos al proyecto libre.
</commit_message>
<xml_diff>
--- a/tareas.xlsx
+++ b/tareas.xlsx
@@ -49,11 +49,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
+      <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -421,57 +421,142 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="26.29071428571428" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
-    <col width="21.29071428571428" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="26.29071428571428" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="21.29071428571428" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
     <col width="18.29071428571428" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
     <col width="16.86214285714286" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Prueba1</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="n">
-        <v>45544.33278162037</v>
-      </c>
-      <c r="D1" s="3" t="n">
-        <v>45557</v>
-      </c>
-      <c r="E1" t="b">
-        <v>0</v>
+          <t>prueba2</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>17-09-2024</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>25-02-2025</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Prueba2</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>45544.33765436057</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>45619</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
+          <t>Prueba8</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>18-09-2024</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>23-10-2024</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PruebaEditar</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>18-09-2024</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>45591</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Prueba10</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>18-09-2024</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>30-04-2025</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Pruebaaa</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>22-09-2024</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>30-11-2024</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización final del programa y su documentación
</commit_message>
<xml_diff>
--- a/tareas.xlsx
+++ b/tareas.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,6 +561,56 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Prueba nueva</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>20-10-2024</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>22-12-2024</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>20-10-2024</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>22-11-2024</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>